<commit_message>
defore adding distances check
</commit_message>
<xml_diff>
--- a/results_G12/ch2_permation_residue_comb.xlsx
+++ b/results_G12/ch2_permation_residue_comb.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,20 +458,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>131, 781, 781, 1074</t>
+          <t>131, 456, 781, 781, 1074</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>781, 781, 781</t>
+          <t>781</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1661, 1899, 1878</t>
+          <t>1661</t>
         </is>
       </c>
     </row>
@@ -498,7 +498,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>131, 749, 1074, 1106</t>
+          <t>99, 749, 1074, 1106</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -538,7 +538,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>131, 131, 781</t>
+          <t>99, 131, 781</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -562,36 +562,36 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>781, 781, 781, 781, 781, 781, 781, 781, 781, 781, 781, 781, 781</t>
+          <t>781, 781, 781, 781, 781, 781, 781, 781, 781</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1091, 849, 1295, 2065, 2343, 2197, 2309, 2430, 2374, 2385, 2553, 2697, 2734</t>
+          <t>1091, 849, 1295, 2197, 2374, 2385, 2553, 2697, 2734</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>131, 749, 781, 1074, SF</t>
+          <t>99, 456, 749, 781, 1074</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>781, 781, 781</t>
+          <t>781</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>805, 1416, 1331</t>
+          <t>805</t>
         </is>
       </c>
     </row>
@@ -638,7 +638,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>131, 131, 749, 781, 1074</t>
+          <t>99, 131, 749, 781, 1074</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -658,27 +658,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>131, 1074, 1106, SF</t>
+          <t>131, 456, 749, 781, 1074</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1106</t>
+          <t>781, 781, 781</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1489</t>
+          <t>1416, 1331, 6643</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>99, 749, 781, 1074</t>
+          <t>99, 781, 1074, SF</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -691,34 +691,34 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1585</t>
+          <t>1489</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>131, 749, 1074, 1106, SF</t>
+          <t>99, 131, 749, 1074</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1106</t>
+          <t>131, 131</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1638</t>
+          <t>1585, 2537</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>749, 749, 781, 1074</t>
+          <t>99, 781, 781, 1074</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -731,94 +731,94 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1811</t>
+          <t>1899</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>749, 781, 1074</t>
+          <t>99, 456, 749, 1074, 1106</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>781, 781</t>
+          <t>1106</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1842, 4719</t>
+          <t>1638</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>131, 131, 749, 1074</t>
+          <t>749, 749, 781, 1074</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>131, 131</t>
+          <t>781</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2151, 2605</t>
+          <t>1811</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>131, 456, 781, 1074</t>
+          <t>456, 749, 781, 1074</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>781, 456</t>
+          <t>781</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2079, 1940</t>
+          <t>1842</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>131, 749, 781, 781</t>
+          <t>99, 131, 749, 1074, SF</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>781</t>
+          <t>131, 131</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1988</t>
+          <t>2151, 2065</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>131, 131, 781, SF</t>
+          <t>99, 131, 781, 1074</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -826,19 +826,19 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>781</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2113</t>
+          <t>2079</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>131, 456, 749, 781</t>
+          <t>131, 781, 781, 1074</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -846,19 +846,19 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>781</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>3680</t>
+          <t>1878</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>131, 749, 781, 1106</t>
+          <t>131, 131, 781, 1074</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -866,59 +866,59 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>781</t>
+          <t>131</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2241</t>
+          <t>1940</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>131, 131, 749, 1106</t>
+          <t>131, 749, 781, 781</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>131, 131</t>
+          <t>781</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2537, 4695</t>
+          <t>1988</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>131, 781, 1074</t>
+          <t>99, 749, 781, 1074</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>781</t>
+          <t>781, 781, 781</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2833</t>
+          <t>2343, 2309, 2430</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>131, 781, 781, 1106</t>
+          <t>99, 456, 781, 781</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -931,14 +931,14 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2474</t>
+          <t>2113</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>131, 424, 781, 1106</t>
+          <t>131, 456, 749, 781</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -946,79 +946,79 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>781</t>
+          <t>456</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>4010</t>
+          <t>3680</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>99, 749, 781</t>
+          <t>99, 749, 781, 1106</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>781</t>
+          <t>781, 781</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>3008</t>
+          <t>2241, 5636</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>131, 749, 781</t>
+          <t>99, 781, 1074</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>781, 781</t>
+          <t>781</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>3280, 3394</t>
+          <t>2833</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>131, 456, 1106</t>
+          <t>131, 131, 781, 1106</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>456, 131</t>
+          <t>781</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>3861, 4290</t>
+          <t>2474</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>131, 781, 1074, 1106</t>
+          <t>131, 424, 781, 1106</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1031,14 +1031,14 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3903</t>
+          <t>4010</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>131, 424, 456, 781</t>
+          <t>131, 131, 749, 1074</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1046,19 +1046,19 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>131</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>4047</t>
+          <t>2605</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>131, 456, 456, 1106</t>
+          <t>99, 749, 781</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1066,59 +1066,59 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>781</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>4907</t>
+          <t>3008</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>456, 749, 1074, 1106</t>
+          <t>131, 749, 781</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>781, 781</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>4062</t>
+          <t>3280, 3394</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>456, 749, 1106</t>
+          <t>131, 456, 1106</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>456, 131, 1106</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>4414</t>
+          <t>3861, 4290, 5791</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>131, 424, 781, 1074</t>
+          <t>131, 131, 1074, 1106</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1126,19 +1126,19 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>781</t>
+          <t>131</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>4508</t>
+          <t>3903</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>99, 424, 456, 781, 1074</t>
+          <t>749, 781, 1074</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1146,59 +1146,59 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>781</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>5470</t>
+          <t>4719</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>131, 456, 749, 1074</t>
+          <t>131, 424, 456, 749</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>456, 456</t>
+          <t>456</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>4624, 6582</t>
+          <t>4047</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>131, 424, 456, 749, 1074</t>
+          <t>131, 131, 1106, 1106</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>456, 456</t>
+          <t>131</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>4577, 5223</t>
+          <t>4907</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>99, 749, SF</t>
+          <t>131, 749, 1074, 1106</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1206,19 +1206,19 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>131</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>5704</t>
+          <t>4062</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>99, 749, 781, 1106</t>
+          <t>456, 749, 1106</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1226,19 +1226,19 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>781</t>
+          <t>456</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>5636</t>
+          <t>4414</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>456, 749, 781, 1106, SF</t>
+          <t>131, 424, 781, 1074</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1246,19 +1246,19 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>781</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>5100</t>
+          <t>4508</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>99, 781, 1074, 1074</t>
+          <t>99, 424, 456, 781, 1074</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1266,19 +1266,19 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>781</t>
+          <t>456</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>5275</t>
+          <t>5470</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>131, 424, 456, 456, 749, 1074</t>
+          <t>99, 456, 749, 1074</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1291,14 +1291,14 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>4991</t>
+          <t>4624</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>131, 424, 456, 749, 781, 1074</t>
+          <t>131, 424, 456, 749, 1074</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1311,14 +1311,14 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>5030</t>
+          <t>4577</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>131, 456, 749, 781, 1074</t>
+          <t>131, 131, 749, 1106</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1326,19 +1326,19 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>131</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>5124</t>
+          <t>4695</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>99, 781, 1074, SF</t>
+          <t>99, 99, 749</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1346,19 +1346,19 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>781</t>
+          <t>99</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>5477</t>
+          <t>5704</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>456, 781, 1106</t>
+          <t>99, 456, 749, 781, 1106, SF</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1366,19 +1366,19 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1106</t>
+          <t>456</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>5791</t>
+          <t>5100</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>99, 781, 1074, 1074</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1386,19 +1386,19 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>781</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>5858</t>
+          <t>5275</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>131, 1106</t>
+          <t>99, 424, 456, 456, 749, 1074</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1406,19 +1406,19 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1106</t>
+          <t>456</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>5837</t>
+          <t>4991</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>99, 424, 456, 749, 781, 1074</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1426,19 +1426,19 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>456</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>5872</t>
+          <t>5030</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>781, 781</t>
+          <t>131, 749, 781, 1074, 1106</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1446,19 +1446,19 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>781</t>
+          <t>1106</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>6040</t>
+          <t>5124</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>456, 456</t>
+          <t>99, 131, 424, 456, 1074</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1471,34 +1471,34 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>5964</t>
+          <t>5223</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>424, 749, 1106</t>
+          <t>99, 424, 781, 1074</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>1106, 424, 749</t>
+          <t>781</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>6798, 6798, 6798</t>
+          <t>5477</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>456, 1074</t>
+          <t>424, 456</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1511,14 +1511,14 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>6080</t>
+          <t>5858</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>456, 456, 1074</t>
+          <t>131, 1106</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1526,19 +1526,19 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>1106</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>6152</t>
+          <t>5837</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>99, 456, 1074</t>
+          <t>131</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1546,19 +1546,19 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>131</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>6176</t>
+          <t>5872</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>99, 456, 781, 1074</t>
+          <t>781, 1106</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1571,14 +1571,14 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>6643</t>
+          <t>6040</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>424, 456, 1074</t>
+          <t>456, 456</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1591,34 +1591,34 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>6231</t>
+          <t>5964</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>424, 456, 749, 1106</t>
+          <t>424, 749, 1106</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>456</t>
+          <t>1106, 424, 749</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>6334</t>
+          <t>6798, 6798, 6798</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>456, 456, 749, 1074</t>
+          <t>456, 1074</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1631,14 +1631,14 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>6452</t>
+          <t>6080</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>424, 456, 749, 1074</t>
+          <t>456, 456, 1074</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1651,34 +1651,34 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>6466</t>
+          <t>6152</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>424, 749, 781, 1106</t>
+          <t>99, 456, 1074</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>781, 781</t>
+          <t>456</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>6503, 6532</t>
+          <t>6176</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>99, 456, 1106, SF</t>
+          <t>424, 456, 1074</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1690,6 +1690,126 @@
         </is>
       </c>
       <c r="D63" t="inlineStr">
+        <is>
+          <t>6231</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>424, 456, 749, 1106, SF</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>6334</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>456, 456, 781, 1074</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>1</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>6452</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>424, 456, 749, 1074</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>1</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>6466</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>424, 749, 781, 1106</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>2</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>781, 781</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>6503, 6532</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>131, 456, 749, 1074</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>456</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>6582</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>99, 131, 456, 1106</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>1</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>131</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
         <is>
           <t>6737</t>
         </is>

</xml_diff>